<commit_message>
Updated tests to run with new version of FORCING classes
</commit_message>
<xml_diff>
--- a/results/test_GROUND_fcSimple_salt_seb/test_GROUND_fcSimple_salt_seb.xlsx
+++ b/results/test_GROUND_fcSimple_salt_seb/test_GROUND_fcSimple_salt_seb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thin\02_Code\Matlab\CryoGRID\2021-0605_CryoGrid\CryoGridTesting\results\test_GROUND_fcSimple_salt_seb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76555CE9-B197-48D2-9673-BED5B87DE6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBD5FE8-AAD8-4BA5-AB33-0539D4ABAFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>end_time</t>
   </si>
   <si>
-    <t>FORCING_seb</t>
-  </si>
-  <si>
     <t>STRAT_layers</t>
   </si>
   <si>
@@ -508,6 +505,9 @@
   </si>
   <si>
     <t>xlsx</t>
+  </si>
+  <si>
+    <t>FORCING_seb_old</t>
   </si>
 </sst>
 </file>
@@ -559,15 +559,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -851,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +864,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>14</v>
@@ -876,35 +872,32 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -913,7 +906,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -924,21 +917,21 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
         <v>102</v>
       </c>
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -977,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,217 +984,207 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>104</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
         <v>42</v>
       </c>
-      <c r="F16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
         <v>112</v>
       </c>
-      <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>134</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-    </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>31</v>
@@ -1212,7 +1195,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>14</v>
@@ -1220,7 +1203,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
@@ -1228,55 +1211,55 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39">
         <v>0.25</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" t="s">
+        <v>159</v>
+      </c>
+      <c r="D42" t="s">
         <v>140</v>
-      </c>
-      <c r="B42" t="s">
-        <v>160</v>
-      </c>
-      <c r="D42" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,7 +1269,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>14</v>
@@ -1294,7 +1277,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B46" s="2">
         <v>1</v>
@@ -1302,7 +1285,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -1331,7 +1314,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
@@ -1342,64 +1325,64 @@
         <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>40</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="5">
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58">
         <v>2011</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58">
         <v>8</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58">
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>41</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C59" s="5">
+      <c r="B59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59">
         <v>2012</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59">
         <v>8</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59">
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,7 +1449,7 @@
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,7 +1463,7 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,12 +1477,12 @@
         <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -1508,7 +1491,7 @@
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1514,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" s="2">
         <v>1</v>
@@ -1539,10 +1522,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" t="s">
         <v>119</v>
-      </c>
-      <c r="B74" t="s">
-        <v>120</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>23</v>
@@ -1554,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,7 +1630,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,7 +1640,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>14</v>
@@ -1665,7 +1648,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B87" s="2">
         <v>1</v>
@@ -1673,19 +1656,19 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" t="s">
         <v>122</v>
       </c>
-      <c r="B89" t="s">
-        <v>123</v>
-      </c>
       <c r="C89" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89" t="s">
         <v>66</v>
       </c>
-      <c r="D89" t="s">
-        <v>67</v>
-      </c>
       <c r="E89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -1704,7 +1687,7 @@
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -1712,57 +1695,51 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" s="4"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>159</v>
-      </c>
-      <c r="C94" s="7"/>
+        <v>158</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>68</v>
-      </c>
-      <c r="B95" s="4">
-        <v>1</v>
-      </c>
-      <c r="C95" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B96" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -1772,7 +1749,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>14</v>
@@ -1780,7 +1757,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B101" s="2">
         <v>1</v>
@@ -1788,10 +1765,10 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B103" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>33</v>
@@ -1803,22 +1780,22 @@
         <v>20</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I103" t="s">
+        <v>144</v>
+      </c>
+      <c r="J103" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J103" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="K103" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -1843,7 +1820,7 @@
       <c r="H104">
         <v>0</v>
       </c>
-      <c r="I104" s="8">
+      <c r="I104" s="4">
         <v>600</v>
       </c>
       <c r="J104">
@@ -1873,7 +1850,7 @@
       <c r="H105">
         <v>0</v>
       </c>
-      <c r="I105" s="8">
+      <c r="I105" s="4">
         <v>0</v>
       </c>
       <c r="J105">
@@ -1883,7 +1860,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -1891,24 +1868,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
-      <c r="C109" s="7"/>
-    </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C110" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B111" s="2">
         <v>1</v>
@@ -1916,16 +1889,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D113" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -1970,7 +1943,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -1985,31 +1958,25 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B124" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C124" s="5"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B125" s="6">
-        <v>1</v>
-      </c>
-      <c r="C125" s="5"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
+        <v>146</v>
+      </c>
+      <c r="B125" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="5" t="s">
+      <c r="B127" t="s">
         <v>15</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C127" t="s">
         <v>16</v>
       </c>
       <c r="D127" t="s">
@@ -2020,10 +1987,10 @@
       <c r="A128" t="s">
         <v>1</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128">
         <v>0.15</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C128">
         <v>0.15</v>
       </c>
       <c r="D128" t="s">
@@ -2037,10 +2004,10 @@
       <c r="A129" t="s">
         <v>2</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B129">
         <v>0.99</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C129">
         <v>0.99</v>
       </c>
       <c r="D129" t="s">
@@ -2052,7 +2019,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B130">
         <v>100</v>
@@ -2064,17 +2031,17 @@
         <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131">
         <v>1E-3</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C131">
         <v>1E-3</v>
       </c>
       <c r="D131" t="s">
@@ -2084,34 +2051,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="5"/>
-      <c r="C132" s="5"/>
-    </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>48</v>
-      </c>
-      <c r="B133" s="5">
+        <v>47</v>
+      </c>
+      <c r="B133">
         <v>3600</v>
       </c>
-      <c r="C133" s="5"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>49</v>
-      </c>
-      <c r="B134" s="5">
+        <v>48</v>
+      </c>
+      <c r="B134">
         <v>50000</v>
       </c>
-      <c r="C134" s="5"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>32</v>
       </c>
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
@@ -2123,28 +2082,25 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B138" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B139" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="B139" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B141" s="5" t="s">
+      <c r="B141" t="s">
         <v>15</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C141" t="s">
         <v>16</v>
       </c>
       <c r="D141" t="s">
@@ -2155,10 +2111,10 @@
       <c r="A142" t="s">
         <v>1</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142">
         <v>0.15</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C142">
         <v>0.15</v>
       </c>
       <c r="D142" t="s">
@@ -2172,10 +2128,10 @@
       <c r="A143" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143">
         <v>0.99</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C143">
         <v>0.99</v>
       </c>
       <c r="D143" t="s">
@@ -2189,10 +2145,10 @@
       <c r="A144" t="s">
         <v>3</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144">
         <v>1E-3</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C144">
         <v>1E-3</v>
       </c>
       <c r="D144" t="s">
@@ -2204,21 +2160,20 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>65</v>
-      </c>
-      <c r="B145" s="5">
+        <v>64</v>
+      </c>
+      <c r="B145">
         <v>100</v>
       </c>
-      <c r="C145" s="5"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>0</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" t="s">
         <v>0</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" t="s">
         <v>0</v>
       </c>
       <c r="E146" t="s">
@@ -2227,12 +2182,12 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>48</v>
-      </c>
-      <c r="B147" s="5">
+        <v>47</v>
+      </c>
+      <c r="B147">
         <v>3600</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C147">
         <v>3600</v>
       </c>
       <c r="D147" t="s">
@@ -2244,12 +2199,12 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>49</v>
-      </c>
-      <c r="B148" s="5">
+        <v>48</v>
+      </c>
+      <c r="B148">
         <v>50000</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C148">
         <v>50000</v>
       </c>
       <c r="D148" t="s">
@@ -2263,46 +2218,33 @@
       <c r="A149" t="s">
         <v>32</v>
       </c>
-      <c r="B149" s="5"/>
-      <c r="C149" s="5"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="5"/>
-      <c r="C150" s="5"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C151" s="5"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B152" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C152" s="5"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B153" s="6">
-        <v>1</v>
-      </c>
-      <c r="C153" s="5"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="5"/>
-      <c r="C154" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="B153" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="5" t="s">
+      <c r="B155" t="s">
         <v>15</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C155" t="s">
         <v>16</v>
       </c>
       <c r="D155" t="s">
@@ -2313,10 +2255,10 @@
       <c r="A156" t="s">
         <v>1</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156">
         <v>0.15</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C156">
         <v>0.15</v>
       </c>
       <c r="D156" t="s">
@@ -2330,10 +2272,10 @@
       <c r="A157" t="s">
         <v>2</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157">
         <v>0.99</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C157">
         <v>0.99</v>
       </c>
       <c r="D157" t="s">
@@ -2345,7 +2287,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B158">
         <v>100</v>
@@ -2357,17 +2299,17 @@
         <v>5</v>
       </c>
       <c r="E158" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>3</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159">
         <v>1E-3</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C159">
         <v>1E-3</v>
       </c>
       <c r="D159" t="s">
@@ -2379,7 +2321,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B160">
         <v>1.5</v>
@@ -2391,61 +2333,46 @@
         <v>5</v>
       </c>
       <c r="E160" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="5"/>
-      <c r="C161" s="5"/>
+        <v>149</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>48</v>
-      </c>
-      <c r="B162" s="5">
+        <v>47</v>
+      </c>
+      <c r="B162">
         <v>3600</v>
       </c>
-      <c r="C162" s="5"/>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>49</v>
-      </c>
-      <c r="B163" s="5">
+        <v>48</v>
+      </c>
+      <c r="B163">
         <v>50000</v>
       </c>
-      <c r="C163" s="5"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>32</v>
       </c>
-      <c r="B164" s="5"/>
-      <c r="C164" s="5"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="5"/>
-      <c r="C165" s="5"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>21</v>
       </c>
-      <c r="B166" s="5"/>
-      <c r="C166" s="5"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B167" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C167" s="5"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B168" s="2">
         <v>1</v>
@@ -2464,7 +2391,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B171">
         <v>300</v>
@@ -2473,15 +2400,15 @@
         <v>350</v>
       </c>
       <c r="D171" t="s">
+        <v>151</v>
+      </c>
+      <c r="E171" t="s">
         <v>152</v>
-      </c>
-      <c r="E171" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B172">
         <v>0.85</v>
@@ -2493,12 +2420,12 @@
         <v>5</v>
       </c>
       <c r="E172" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B173">
         <v>0.55000000000000004</v>
@@ -2510,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="E173" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="E177" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -2597,7 +2524,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B179">
         <v>3600</v>
@@ -2614,7 +2541,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B180">
         <v>50000</v>
@@ -2631,7 +2558,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B181">
         <v>0.01</v>
@@ -2643,7 +2570,7 @@
         <v>6</v>
       </c>
       <c r="E181" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -2651,44 +2578,32 @@
         <v>32</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B183" s="5"/>
-      <c r="C183" s="5"/>
-    </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>21</v>
       </c>
-      <c r="B184" s="5"/>
-      <c r="C184" s="5"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B185" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C185" s="5"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B186" s="6">
-        <v>1</v>
-      </c>
-      <c r="C186" s="5"/>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B187" s="5"/>
-      <c r="C187" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B186" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B188" s="5" t="s">
+      <c r="B188" t="s">
         <v>15</v>
       </c>
-      <c r="C188" s="5" t="s">
+      <c r="C188" t="s">
         <v>16</v>
       </c>
       <c r="D188" t="s">
@@ -2697,19 +2612,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>77</v>
-      </c>
-      <c r="B189" s="5">
+        <v>76</v>
+      </c>
+      <c r="B189">
         <v>0.25</v>
       </c>
-      <c r="C189" s="5"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>32</v>
       </c>
-      <c r="B190" s="5"/>
-      <c r="C190" s="5"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
@@ -2718,7 +2630,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>14</v>
@@ -2726,7 +2638,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -2745,7 +2657,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>